<commit_message>
ADS example + ADS code reading vars
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Nicky Verhees.xlsx
+++ b/Algemeen/Logboek/Logboek Nicky Verhees.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Proftaak S4\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AE8B45-6FD0-4DF8-ABFB-6422493E4BDC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D5BA32-287F-4138-8316-8F4C215F5334}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,20 +753,20 @@
         <v>5</v>
       </c>
       <c r="D10" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="10">
         <f xml:space="preserve"> D10 - B10- F10</f>
-        <v>-9</v>
+        <v>5</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>5</v>
@@ -815,26 +815,26 @@
         <v>12</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>5</v>
@@ -1190,28 +1190,28 @@
       </c>
       <c r="B23" s="5">
         <f>B4 + B5 + B6 + B7 + B8 + B9 + B11 + B12 + B13 + B14 + B15 + B16 + B17 + B18 + B19 + B20 + B21 + B22</f>
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="6">
         <f>D4 + D5 + D6 + D7 + D8 + D9 + D10 + D11 + D12 + D13 + D14 + D15 + D16 + D17 + D18 + D19 + D20 + D21 + D22</f>
-        <v>89.5</v>
+        <v>119.5</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5">
         <f>F4 + F5 + F6 + F7 + F8 + F9 + F10 + F11 + F12 + F13 + F14+ F15 + F16 + F17 + F18 + F19 + F20 + F21 + F22</f>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="7">
         <f xml:space="preserve"> H4 + H5 + H6 + H7 + H8 + H9 + H10 + H11 + H12 + H13 + H14 + H15 + H16 + H17 + H18 + H19 + H20 + H21 + H22</f>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
ADS application update + logboek
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Nicky Verhees.xlsx
+++ b/Algemeen/Logboek/Logboek Nicky Verhees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Proftaak S4\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D5BA32-287F-4138-8316-8F4C215F5334}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4975E5-AC7B-425F-9514-BD2A305AE56D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -470,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78840537-239C-47B0-A4CC-46A5360523B1}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,26 +748,26 @@
         <v>10</v>
       </c>
       <c r="B10" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="10">
         <f xml:space="preserve"> D10 - B10- F10</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>5</v>
@@ -781,26 +782,26 @@
         <v>11</v>
       </c>
       <c r="B11" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="9">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" ref="H11:H19" si="0" xml:space="preserve"> D11 - B11 - F11</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>5</v>
@@ -821,13 +822,13 @@
         <v>5</v>
       </c>
       <c r="D12" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>5</v>
@@ -1190,28 +1191,28 @@
       </c>
       <c r="B23" s="5">
         <f>B4 + B5 + B6 + B7 + B8 + B9 + B11 + B12 + B13 + B14 + B15 + B16 + B17 + B18 + B19 + B20 + B21 + B22</f>
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="6">
         <f>D4 + D5 + D6 + D7 + D8 + D9 + D10 + D11 + D12 + D13 + D14 + D15 + D16 + D17 + D18 + D19 + D20 + D21 + D22</f>
-        <v>119.5</v>
+        <v>117.5</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5">
         <f>F4 + F5 + F6 + F7 + F8 + F9 + F10 + F11 + F12 + F13 + F14+ F15 + F16 + F17 + F18 + F19 + F20 + F21 + F22</f>
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="7">
         <f xml:space="preserve"> H4 + H5 + H6 + H7 + H8 + H9 + H10 + H11 + H12 + H13 + H14 + H15 + H16 + H17 + H18 + H19 + H20 + H21 + H22</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>5</v>

</xml_diff>